<commit_message>
Conditional Formatting - Red and Green
</commit_message>
<xml_diff>
--- a/ACE_Score_Calculator.xlsx
+++ b/ACE_Score_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B37421-2C4B-4A63-83D7-9D08F558FD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151B512C-0C5F-403D-8493-92146B3E03FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADB8269C-441E-4EA3-BBFF-0F70A78339A0}"/>
   </bookViews>
@@ -386,8 +386,76 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -698,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3A5406-2839-4F9B-9ACA-EBED87451476}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1176,8 +1244,8 @@
         <v>6.7</v>
       </c>
       <c r="H17" s="28" t="str">
-        <f>IF(B17&lt;G17, "Major impairment", IF(AND(B17&lt;=F17, B17&gt;=G17), "Minor impairment", "No impairments"))</f>
-        <v>Major impairment</v>
+        <f>IF(B17&lt;G17, "Major Impairment", IF(AND(B17&lt;=F17, B17&gt;=G17), "Minor Impairment", "No Impairments"))</f>
+        <v>Major Impairment</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1208,8 +1276,8 @@
         <v>3.4</v>
       </c>
       <c r="H18" s="28" t="str">
-        <f>IF(B18&lt;G18, "Major impairment", IF(AND(B18&lt;=F18, B18&gt;=G18), "Minor impairment", "No impairments"))</f>
-        <v>Major impairment</v>
+        <f t="shared" ref="H18:H25" si="5">IF(B18&lt;G18, "Major Impairment", IF(AND(B18&lt;=F18, B18&gt;=G18), "Minor Impairment", "No Impairments"))</f>
+        <v>Major Impairment</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1240,8 +1308,8 @@
         <v>13.700000000000001</v>
       </c>
       <c r="H19" s="28" t="str">
-        <f t="shared" ref="H19:H25" si="5">IF(B19&lt;G19, "Major impairment", IF(AND(B19&lt;=F19, B19&gt;=G19), "Minor impairment", "No impairments"))</f>
-        <v>Major impairment</v>
+        <f t="shared" si="5"/>
+        <v>Major Impairment</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1273,7 +1341,7 @@
       </c>
       <c r="H20" s="28" t="str">
         <f t="shared" si="5"/>
-        <v>No impairments</v>
+        <v>No Impairments</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1305,7 +1373,7 @@
       </c>
       <c r="H21" s="28" t="str">
         <f t="shared" si="5"/>
-        <v>Major impairment</v>
+        <v>Major Impairment</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1337,7 +1405,7 @@
       </c>
       <c r="H22" s="28" t="str">
         <f t="shared" si="5"/>
-        <v>No impairments</v>
+        <v>No Impairments</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1369,7 +1437,7 @@
       </c>
       <c r="H23" s="28" t="str">
         <f t="shared" si="5"/>
-        <v>No impairments</v>
+        <v>No Impairments</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1401,7 +1469,7 @@
       </c>
       <c r="H24" s="28" t="str">
         <f t="shared" si="5"/>
-        <v>Major impairment</v>
+        <v>Major Impairment</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1433,10 +1501,18 @@
       </c>
       <c r="H25" s="28" t="str">
         <f t="shared" si="5"/>
-        <v>No impairments</v>
+        <v>No Impairments</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B17:B25">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$H17="No Impairments"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$H17="Major impairment"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Conditional Formatting - Yellow
</commit_message>
<xml_diff>
--- a/ACE_Score_Calculator.xlsx
+++ b/ACE_Score_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151B512C-0C5F-403D-8493-92146B3E03FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0226ED5-FE68-4A79-847A-6EB105875286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADB8269C-441E-4EA3-BBFF-0F70A78339A0}"/>
   </bookViews>
@@ -386,7 +386,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -398,7 +398,14 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FFFFCC00"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -414,6 +421,21 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFFCC00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -767,7 +789,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,7 +1235,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="24">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1225,27 +1247,27 @@
       </c>
       <c r="C17">
         <f>IF($B$16=0,B4,IF($B$16&lt;=4,C4,IF($B$16&lt;=8,D4,IF($B$16&lt;=12,E4,F4))))</f>
-        <v>7.9</v>
+        <v>7.7</v>
       </c>
       <c r="D17">
         <f>IF($B$16=0,H4,IF($B$16&lt;=4,I4,IF($B$16&lt;=8,J4,IF($B$16&lt;=12,K4,L4))))</f>
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="E17">
         <f>IF($B$16=0,H4,IF($B$16&lt;=4,I4,IF($B$16&lt;=8,J4,IF($B$16&lt;=12,K4,L4))))*2</f>
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F17">
         <f>C17-D17</f>
-        <v>7.3000000000000007</v>
+        <v>6.8</v>
       </c>
       <c r="G17">
         <f>C17-E17</f>
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="H17" s="28" t="str">
         <f>IF(B17&lt;G17, "Major Impairment", IF(AND(B17&lt;=F17, B17&gt;=G17), "Minor Impairment", "No Impairments"))</f>
-        <v>Major Impairment</v>
+        <v>Minor Impairment</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1257,23 +1279,23 @@
       </c>
       <c r="C18">
         <f t="shared" ref="C18:C25" si="0">IF($B$16=0,B5,IF($B$16&lt;=4,C5,IF($B$16&lt;=8,D5,IF($B$16&lt;=12,E5,F5))))</f>
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D25" si="1">IF($B$16=0,H5,IF($B$16&lt;=4,I5,IF($B$16&lt;=8,J5,IF($B$16&lt;=12,K5,L5))))</f>
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E18">
         <f t="shared" ref="E18:E25" si="2">IF($B$16=0,H5,IF($B$16&lt;=4,I5,IF($B$16&lt;=8,J5,IF($B$16&lt;=12,K5,L5))))*2</f>
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F25" si="3">C18-D18</f>
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G25" si="4">C18-E18</f>
-        <v>3.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H18" s="28" t="str">
         <f t="shared" ref="H18:H25" si="5">IF(B18&lt;G18, "Major Impairment", IF(AND(B18&lt;=F18, B18&gt;=G18), "Minor Impairment", "No Impairments"))</f>
@@ -1289,23 +1311,23 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>20.100000000000001</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>4.3</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>6.4</v>
+        <v>8.6</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>16.900000000000002</v>
+        <v>13.8</v>
       </c>
       <c r="G19">
         <f>C19-E19</f>
-        <v>13.700000000000001</v>
+        <v>9.5000000000000018</v>
       </c>
       <c r="H19" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1321,23 +1343,23 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>7.2</v>
+        <v>6.2</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>3.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>5.3000000000000007</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="G20">
         <f t="shared" si="4"/>
-        <v>3.4000000000000004</v>
+        <v>1.6000000000000005</v>
       </c>
       <c r="H20" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1353,23 +1375,23 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="H21" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1385,23 +1407,23 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>8.9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>7.4</v>
+        <v>6.2</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="G22">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>2.1000000000000005</v>
       </c>
       <c r="H22" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1417,23 +1439,23 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>10.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <v>5.2</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>8.6000000000000014</v>
+        <v>7.2000000000000011</v>
       </c>
       <c r="G23">
         <f t="shared" si="4"/>
-        <v>6.4</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="H23" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1449,23 +1471,23 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>15.7</v>
+        <v>15.6</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
-        <v>14.799999999999999</v>
+        <v>14.6</v>
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>13.899999999999999</v>
+        <v>13.6</v>
       </c>
       <c r="H24" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1481,23 +1503,23 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>2.1999999999999997</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="G25">
         <f t="shared" si="4"/>
-        <v>0.59999999999999964</v>
+        <v>-0.80000000000000027</v>
       </c>
       <c r="H25" s="28" t="str">
         <f t="shared" si="5"/>
@@ -1506,11 +1528,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B17:B25">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>$H17="No Impairments"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$H17="Major impairment"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$H17="Minor Impairment"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1522,8 +1547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863541EE-4AEB-41E9-9928-651CDE0E540A}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1968,7 +1993,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="24">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1980,27 +2005,27 @@
       </c>
       <c r="C17">
         <f>IF($B$16=0,B4,IF($B$16&lt;=4,C4,IF($B$16&lt;=8,D4,IF($B$16&lt;=12,E4,F4))))</f>
-        <v>7.9</v>
+        <v>7.7</v>
       </c>
       <c r="D17">
         <f>IF($B$16=0,H4,IF($B$16&lt;=4,I4,IF($B$16&lt;=8,J4,IF($B$16&lt;=12,K4,L4))))</f>
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="E17">
         <f>IF($B$16=0,H4,IF($B$16&lt;=4,I4,IF($B$16&lt;=8,J4,IF($B$16&lt;=12,K4,L4))))*2</f>
-        <v>1.2</v>
+        <v>1.8</v>
       </c>
       <c r="F17">
         <f>C17-D17</f>
-        <v>7.3000000000000007</v>
+        <v>6.8</v>
       </c>
       <c r="G17">
         <f>C17-E17</f>
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="H17" t="str">
         <f>IF(B17&lt;G17, "Major impairment", IF(AND(B17&lt;=F17, B17&gt;=G17), "Minor impairment", "No impairments"))</f>
-        <v>Major impairment</v>
+        <v>Minor impairment</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2012,23 +2037,23 @@
       </c>
       <c r="C18">
         <f t="shared" ref="C18:C25" si="0">IF($B$16=0,B5,IF($B$16&lt;=4,C5,IF($B$16&lt;=8,D5,IF($B$16&lt;=12,E5,F5))))</f>
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="D18">
         <f t="shared" ref="D18:D25" si="1">IF($B$16=0,H5,IF($B$16&lt;=4,I5,IF($B$16&lt;=8,J5,IF($B$16&lt;=12,K5,L5))))</f>
-        <v>0.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E18">
         <f t="shared" ref="E18:E25" si="2">IF($B$16=0,H5,IF($B$16&lt;=4,I5,IF($B$16&lt;=8,J5,IF($B$16&lt;=12,K5,L5))))*2</f>
-        <v>1.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F18">
         <f t="shared" ref="F18:F25" si="3">C18-D18</f>
-        <v>4.0999999999999996</v>
+        <v>3.4</v>
       </c>
       <c r="G18">
         <f t="shared" ref="G18:G25" si="4">C18-E18</f>
-        <v>3.4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H18" t="str">
         <f>IF(B18&lt;G18, "Major impairment", IF(AND(B18&lt;=F18, B18&gt;=G18), "Minor impairment", "No impairments"))</f>
@@ -2044,23 +2069,23 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>20.100000000000001</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>3.2</v>
+        <v>4.3</v>
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>6.4</v>
+        <v>8.6</v>
       </c>
       <c r="F19">
         <f t="shared" si="3"/>
-        <v>16.900000000000002</v>
+        <v>13.8</v>
       </c>
       <c r="G19">
         <f>C19-E19</f>
-        <v>13.700000000000001</v>
+        <v>9.5000000000000018</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" ref="H19:H25" si="5">IF(B19&lt;G19, "Major impairment", IF(AND(B19&lt;=F19, B19&gt;=G19), "Minor impairment", "No impairments"))</f>
@@ -2076,23 +2101,23 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>7.2</v>
+        <v>6.2</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>1.9</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>3.8</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F20">
         <f t="shared" si="3"/>
-        <v>5.3000000000000007</v>
+        <v>3.9000000000000004</v>
       </c>
       <c r="G20">
         <f t="shared" si="4"/>
-        <v>3.4000000000000004</v>
+        <v>1.6000000000000005</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="5"/>
@@ -2108,23 +2133,23 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>3.5</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>1.4</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="G21">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="5"/>
@@ -2140,23 +2165,23 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>8.9</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>3.7</v>
+        <v>3.1</v>
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>7.4</v>
+        <v>6.2</v>
       </c>
       <c r="F22">
         <f t="shared" si="3"/>
-        <v>5.2</v>
+        <v>5.2000000000000011</v>
       </c>
       <c r="G22">
         <f t="shared" si="4"/>
-        <v>1.5</v>
+        <v>2.1000000000000005</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="5"/>
@@ -2172,23 +2197,23 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>10.8</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <v>5.2</v>
       </c>
       <c r="F23">
         <f t="shared" si="3"/>
-        <v>8.6000000000000014</v>
+        <v>7.2000000000000011</v>
       </c>
       <c r="G23">
         <f t="shared" si="4"/>
-        <v>6.4</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="5"/>
@@ -2204,23 +2229,23 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>15.7</v>
+        <v>15.6</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="F24">
         <f t="shared" si="3"/>
-        <v>14.799999999999999</v>
+        <v>14.6</v>
       </c>
       <c r="G24">
         <f t="shared" si="4"/>
-        <v>13.899999999999999</v>
+        <v>13.6</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="5"/>
@@ -2236,23 +2261,23 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>2.8</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="F25">
         <f t="shared" si="3"/>
-        <v>2.1999999999999997</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="G25">
         <f t="shared" si="4"/>
-        <v>0.59999999999999964</v>
+        <v>-0.80000000000000027</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="5"/>
@@ -2269,7 +2294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6B59A-51EC-41AF-94B1-B924BC983D74}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Read only and input cells demarcation
</commit_message>
<xml_diff>
--- a/ACE_Score_Calculator.xlsx
+++ b/ACE_Score_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E490A08-94FB-45AE-9BED-A637766FEFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FC0EA4-8797-42A0-8DA9-712F38B977C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADB8269C-441E-4EA3-BBFF-0F70A78339A0}"/>
   </bookViews>
@@ -431,9 +431,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="1" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3A5406-2839-4F9B-9ACA-EBED87451476}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,7 +1243,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>46</v>
@@ -1261,7 +1263,7 @@
       </c>
       <c r="C18" s="27">
         <f t="shared" ref="C18:C26" si="0">IF($B$17=0,B4,IF($B$17&lt;=4,C4,IF($B$17&lt;=8,D4,IF($B$17&lt;=12,E4,F4))))</f>
-        <v>3.9</v>
+        <v>6.6</v>
       </c>
       <c r="D18" s="27">
         <f t="shared" ref="D18:D26" si="1">IF($B$17=0,H4,IF($B$17&lt;=4,I4,IF($B$17&lt;=8,J4,IF($B$17&lt;=12,K4,L4))))</f>
@@ -1273,11 +1275,11 @@
       </c>
       <c r="F18" s="27">
         <f>C18-D18</f>
-        <v>2.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="G18" s="27">
         <f>C18-E18</f>
-        <v>0.29999999999999982</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="H18" s="29" t="str">
         <f>IF(B18&lt;G18, "Major Impairment", IF(AND(B18&lt;=F18, B18&gt;=G18), "Minor Impairment", "No Impairments"))</f>
@@ -1289,31 +1291,31 @@
         <v>2</v>
       </c>
       <c r="B19" s="34">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19" s="27">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>3.3</v>
       </c>
       <c r="D19" s="27">
         <f t="shared" si="1"/>
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E19" s="27">
         <f t="shared" si="2"/>
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="F19" s="27">
         <f t="shared" ref="F19:F26" si="3">C19-D19</f>
-        <v>9.9999999999999867E-2</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="G19" s="27">
         <f t="shared" ref="G19:G26" si="4">C19-E19</f>
-        <v>-1.2000000000000002</v>
+        <v>0.29999999999999982</v>
       </c>
       <c r="H19" s="29" t="str">
         <f t="shared" ref="H19:H26" si="5">IF(B19&lt;G19, "Major Impairment", IF(AND(B19&lt;=F19, B19&gt;=G19), "Minor Impairment", "No Impairments"))</f>
-        <v>No Impairments</v>
+        <v>Minor Impairment</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1321,31 +1323,31 @@
         <v>3</v>
       </c>
       <c r="B20" s="34">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C20" s="27">
         <f t="shared" si="0"/>
-        <v>10.6</v>
+        <v>14.7</v>
       </c>
       <c r="D20" s="27">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
       <c r="E20" s="27">
         <f t="shared" si="2"/>
-        <v>8.8000000000000007</v>
+        <v>7.8</v>
       </c>
       <c r="F20" s="27">
         <f t="shared" si="3"/>
-        <v>6.1999999999999993</v>
+        <v>10.799999999999999</v>
       </c>
       <c r="G20" s="27">
         <f>C20-E20</f>
-        <v>1.7999999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="H20" s="29" t="str">
         <f t="shared" si="5"/>
-        <v>No Impairments</v>
+        <v>Major Impairment</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1353,31 +1355,31 @@
         <v>4</v>
       </c>
       <c r="B21" s="34">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C21" s="27">
         <f t="shared" si="0"/>
-        <v>3.8</v>
+        <v>4.8</v>
       </c>
       <c r="D21" s="27">
         <f t="shared" si="1"/>
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="E21" s="27">
         <f t="shared" si="2"/>
-        <v>3.8</v>
+        <v>4</v>
       </c>
       <c r="F21" s="27">
         <f t="shared" si="3"/>
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="G21" s="27">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.79999999999999982</v>
       </c>
       <c r="H21" s="29" t="str">
         <f t="shared" si="5"/>
-        <v>Minor Impairment</v>
+        <v>No Impairments</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1385,27 +1387,27 @@
         <v>5</v>
       </c>
       <c r="B22" s="34">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" s="27">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2.6</v>
       </c>
       <c r="D22" s="27">
         <f t="shared" si="1"/>
-        <v>0.9</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E22" s="27">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F22" s="27">
         <f t="shared" si="3"/>
-        <v>9.9999999999999978E-2</v>
+        <v>1.5</v>
       </c>
       <c r="G22" s="27">
         <f t="shared" si="4"/>
-        <v>-0.8</v>
+        <v>0.39999999999999991</v>
       </c>
       <c r="H22" s="29" t="str">
         <f t="shared" si="5"/>
@@ -1417,27 +1419,27 @@
         <v>6</v>
       </c>
       <c r="B23" s="34">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C23" s="27">
         <f t="shared" si="0"/>
-        <v>4.3</v>
+        <v>6.3</v>
       </c>
       <c r="D23" s="27">
         <f t="shared" si="1"/>
-        <v>2.1</v>
+        <v>2.6</v>
       </c>
       <c r="E23" s="27">
         <f t="shared" si="2"/>
-        <v>4.2</v>
+        <v>5.2</v>
       </c>
       <c r="F23" s="27">
         <f t="shared" si="3"/>
-        <v>2.1999999999999997</v>
+        <v>3.6999999999999997</v>
       </c>
       <c r="G23" s="27">
         <f t="shared" si="4"/>
-        <v>9.9999999999999645E-2</v>
+        <v>1.0999999999999996</v>
       </c>
       <c r="H23" s="29" t="str">
         <f t="shared" si="5"/>
@@ -1449,27 +1451,27 @@
         <v>7</v>
       </c>
       <c r="B24" s="34">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C24" s="27">
         <f t="shared" si="0"/>
-        <v>5.2</v>
+        <v>7.6</v>
       </c>
       <c r="D24" s="27">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.9</v>
       </c>
       <c r="E24" s="27">
         <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <v>5.8</v>
       </c>
       <c r="F24" s="27">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4.6999999999999993</v>
       </c>
       <c r="G24" s="27">
         <f t="shared" si="4"/>
-        <v>0.79999999999999982</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="H24" s="29" t="str">
         <f t="shared" si="5"/>
@@ -1481,31 +1483,31 @@
         <v>8</v>
       </c>
       <c r="B25" s="34">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" s="27">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>14.3</v>
       </c>
       <c r="D25" s="27">
         <f t="shared" si="1"/>
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="E25" s="27">
         <f t="shared" si="2"/>
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="F25" s="27">
         <f t="shared" si="3"/>
-        <v>9.6</v>
+        <v>12.5</v>
       </c>
       <c r="G25" s="27">
         <f t="shared" si="4"/>
-        <v>8.1999999999999993</v>
+        <v>10.700000000000001</v>
       </c>
       <c r="H25" s="29" t="str">
         <f t="shared" si="5"/>
-        <v>No Impairments</v>
+        <v>Minor Impairment</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1513,27 +1515,27 @@
         <v>9</v>
       </c>
       <c r="B26" s="34">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C26" s="27">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>1.4</v>
       </c>
       <c r="D26" s="27">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="E26" s="27">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>2.6</v>
       </c>
       <c r="F26" s="27">
         <f t="shared" si="3"/>
-        <v>-0.2</v>
+        <v>9.9999999999999867E-2</v>
       </c>
       <c r="G26" s="27">
         <f t="shared" si="4"/>
-        <v>-0.60000000000000009</v>
+        <v>-1.2000000000000002</v>
       </c>
       <c r="H26" s="29" t="str">
         <f t="shared" si="5"/>
@@ -1581,6 +1583,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="B18:B26">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$H18="Minor Impairment"</formula>
@@ -1607,8 +1610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6B59A-51EC-41AF-94B1-B924BC983D74}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Corrected the Totals calculation
</commit_message>
<xml_diff>
--- a/ACE_Score_Calculator.xlsx
+++ b/ACE_Score_Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vidya\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506D3711-9690-488E-BFD0-821A43682AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E3A847-66BD-43E3-A76D-8E4CD6BB5827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ADB8269C-441E-4EA3-BBFF-0F70A78339A0}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="34">
   <si>
     <t>Total</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>- Cell values in orange indicate minor impairment</t>
+  </si>
+  <si>
+    <t>5. Only cells B17 to B26 are editable.</t>
   </si>
 </sst>
 </file>
@@ -226,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -269,31 +272,23 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3A5406-2839-4F9B-9ACA-EBED87451476}">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,430 +650,430 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="J1"/>
+      <c r="K1"/>
+      <c r="L1"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="19" t="s">
+      <c r="G2"/>
+      <c r="H2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="19" t="s">
+      <c r="J2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="17" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
+      <c r="A3"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="21">
+      <c r="B4" s="4">
         <v>3.9</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="4">
         <v>5.7</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="4">
         <v>6.6</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="4">
         <v>7.7</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="4">
         <v>7.9</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17">
+      <c r="G4"/>
+      <c r="H4">
         <v>1.8</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4">
         <v>1.8</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4">
         <v>1.8</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4">
         <v>0.9</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4">
         <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="4">
         <v>1.4</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="4">
         <v>2.7</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="4">
         <v>3.3</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="4">
         <v>4.5</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="4">
         <v>4.8</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17">
+      <c r="G5"/>
+      <c r="H5">
         <v>1.3</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5">
         <v>1.6</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5">
         <v>1.5</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5">
         <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="4">
         <v>10.6</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="4">
         <v>13.4</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="4">
         <v>14.7</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="4">
         <v>18.100000000000001</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="4">
         <v>20.100000000000001</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17">
+      <c r="G6"/>
+      <c r="H6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6">
         <v>3.9</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6">
         <v>4.3</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6">
         <v>3.2</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="4">
         <v>3.8</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="4">
         <v>4.3</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="4">
         <v>4.8</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="4">
         <v>6.2</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="4">
         <v>7.2</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17">
+      <c r="G7"/>
+      <c r="H7">
         <v>1.9</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7">
         <v>2.1</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7">
         <v>2</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7">
         <v>2.2999999999999998</v>
       </c>
-      <c r="L7" s="17">
+      <c r="L7">
         <v>1.9</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="4">
         <v>1.9</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="4">
         <v>2.6</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="4">
         <v>3.5</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="4">
         <v>3.8</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17">
+      <c r="G8"/>
+      <c r="H8">
         <v>0.9</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8">
         <v>1.2</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8">
         <v>0.7</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8">
         <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="4">
         <v>4.3</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="4">
         <v>5.8</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="4">
         <v>6.3</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="4">
         <v>8.9</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17">
+      <c r="G9"/>
+      <c r="H9">
         <v>2.1</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9">
         <v>2.8</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9">
         <v>2.6</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9">
         <v>3.1</v>
       </c>
-      <c r="L9" s="17">
+      <c r="L9">
         <v>3.7</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="21">
+      <c r="B10" s="4">
         <v>5.2</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="4">
         <v>6.9</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="4">
         <v>7.6</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="4">
         <v>9.8000000000000007</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="4">
         <v>10.8</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17">
+      <c r="G10"/>
+      <c r="H10">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10">
         <v>2.8</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10">
         <v>2.9</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10">
         <v>2.6</v>
       </c>
-      <c r="L10" s="17">
+      <c r="L10">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="4">
         <v>11</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="4">
         <v>13.3</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="4">
         <v>14.3</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="4">
         <v>15.6</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="4">
         <v>15.7</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17">
+      <c r="G11"/>
+      <c r="H11">
         <v>1.4</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11">
         <v>1.8</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11">
         <v>1.8</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11" s="17">
+      <c r="L11">
         <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="4">
         <v>0.2</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="4">
         <v>0.9</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="4">
         <v>1.4</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="4">
         <v>2.8</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="4">
         <v>3.8</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17">
+      <c r="G12"/>
+      <c r="H12">
         <v>0.4</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12">
         <v>1.2</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12">
         <v>1.3</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12">
         <v>1.8</v>
       </c>
-      <c r="L12" s="17">
+      <c r="L12">
         <v>1.6</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="5">
         <v>42.8</v>
       </c>
-      <c r="C13" s="22">
+      <c r="C13" s="5">
         <v>55.9</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="5">
         <v>62.6</v>
       </c>
-      <c r="E13" s="22">
+      <c r="E13" s="5">
         <v>77</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="5">
         <v>83.4</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="22">
+      <c r="G13" s="2"/>
+      <c r="H13" s="5">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="5">
         <v>12.5</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="5">
         <v>11.4</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="5">
         <v>10.199999999999999</v>
       </c>
-      <c r="L13" s="22">
+      <c r="L13" s="5">
         <v>7.2</v>
       </c>
     </row>
@@ -1101,22 +1096,22 @@
       <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="D16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1127,14 +1122,14 @@
       <c r="B17" s="8">
         <v>5</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
@@ -1143,27 +1138,27 @@
       <c r="B18" s="9">
         <v>9</v>
       </c>
-      <c r="C18" s="25">
-        <f t="shared" ref="C18:C26" si="0">IF($B$17=0,B4,IF($B$17&lt;=4,C4,IF($B$17&lt;=8,D4,IF($B$17&lt;=12,E4,F4))))</f>
+      <c r="C18" s="20">
+        <f t="shared" ref="C18:C27" si="0">IF($B$17=0,B4,IF($B$17&lt;=4,C4,IF($B$17&lt;=8,D4,IF($B$17&lt;=12,E4,F4))))</f>
         <v>6.6</v>
       </c>
-      <c r="D18" s="25">
-        <f t="shared" ref="D18:D26" si="1">IF($B$17=0,H4,IF($B$17&lt;=4,I4,IF($B$17&lt;=8,J4,IF($B$17&lt;=12,K4,L4))))</f>
+      <c r="D18" s="20">
+        <f t="shared" ref="D18:D27" si="1">IF($B$17=0,H4,IF($B$17&lt;=4,I4,IF($B$17&lt;=8,J4,IF($B$17&lt;=12,K4,L4))))</f>
         <v>1.8</v>
       </c>
-      <c r="E18" s="25">
-        <f t="shared" ref="E18:E26" si="2">IF($B$17=0,H4,IF($B$17&lt;=4,I4,IF($B$17&lt;=8,J4,IF($B$17&lt;=12,K4,L4))))*2</f>
+      <c r="E18" s="20">
+        <f t="shared" ref="E18:E27" si="2">IF($B$17=0,H4,IF($B$17&lt;=4,I4,IF($B$17&lt;=8,J4,IF($B$17&lt;=12,K4,L4))))*2</f>
         <v>3.6</v>
       </c>
-      <c r="F18" s="25">
+      <c r="F18" s="20">
         <f>C18-D18</f>
         <v>4.8</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="20">
         <f>C18-E18</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="H18" s="26" t="str">
+      <c r="H18" s="21" t="str">
         <f>IF(B18&lt;G18, "Major Impairment", IF(AND(B18&lt;=F18, B18&gt;=G18), "Minor Impairment", "No Impairments"))</f>
         <v>No Impairments</v>
       </c>
@@ -1175,28 +1170,28 @@
       <c r="B19" s="9">
         <v>1</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="20">
         <f t="shared" si="0"/>
         <v>3.3</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="20">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="20">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="F19" s="25">
-        <f t="shared" ref="F19:F26" si="3">C19-D19</f>
+      <c r="F19" s="20">
+        <f t="shared" ref="F19:F27" si="3">C19-D19</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="G19" s="25">
-        <f t="shared" ref="G19:G26" si="4">C19-E19</f>
+      <c r="G19" s="20">
+        <f t="shared" ref="G19:G27" si="4">C19-E19</f>
         <v>0.29999999999999982</v>
       </c>
-      <c r="H19" s="26" t="str">
-        <f t="shared" ref="H19:H26" si="5">IF(B19&lt;G19, "Major Impairment", IF(AND(B19&lt;=F19, B19&gt;=G19), "Minor Impairment", "No Impairments"))</f>
+      <c r="H19" s="21" t="str">
+        <f t="shared" ref="H19:H27" si="5">IF(B19&lt;G19, "Major Impairment", IF(AND(B19&lt;=F19, B19&gt;=G19), "Minor Impairment", "No Impairments"))</f>
         <v>Minor Impairment</v>
       </c>
     </row>
@@ -1207,27 +1202,27 @@
       <c r="B20" s="9">
         <v>9</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="20">
         <f t="shared" si="0"/>
         <v>14.7</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="20">
         <f t="shared" si="1"/>
         <v>3.9</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="20">
         <f t="shared" si="2"/>
         <v>7.8</v>
       </c>
-      <c r="F20" s="25">
+      <c r="F20" s="20">
         <f t="shared" si="3"/>
         <v>10.799999999999999</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="20">
         <f>C20-E20</f>
         <v>6.8999999999999995</v>
       </c>
-      <c r="H20" s="26" t="str">
+      <c r="H20" s="21" t="str">
         <f t="shared" si="5"/>
         <v>Minor Impairment</v>
       </c>
@@ -1239,27 +1234,27 @@
       <c r="B21" s="9">
         <v>5</v>
       </c>
-      <c r="C21" s="25">
+      <c r="C21" s="20">
         <f t="shared" si="0"/>
         <v>4.8</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="20">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="20">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="F21" s="25">
+      <c r="F21" s="20">
         <f t="shared" si="3"/>
         <v>2.8</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="20">
         <f t="shared" si="4"/>
         <v>0.79999999999999982</v>
       </c>
-      <c r="H21" s="26" t="str">
+      <c r="H21" s="21" t="str">
         <f t="shared" si="5"/>
         <v>No Impairments</v>
       </c>
@@ -1271,27 +1266,27 @@
       <c r="B22" s="9">
         <v>1</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="20">
         <f t="shared" si="0"/>
         <v>2.6</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="20">
         <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="20">
         <f t="shared" si="2"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="F22" s="25">
+      <c r="F22" s="20">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="20">
         <f t="shared" si="4"/>
         <v>0.39999999999999991</v>
       </c>
-      <c r="H22" s="26" t="str">
+      <c r="H22" s="21" t="str">
         <f t="shared" si="5"/>
         <v>Minor Impairment</v>
       </c>
@@ -1303,27 +1298,27 @@
       <c r="B23" s="9">
         <v>1</v>
       </c>
-      <c r="C23" s="25">
+      <c r="C23" s="20">
         <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="20">
         <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="20">
         <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
-      <c r="F23" s="25">
+      <c r="F23" s="20">
         <f t="shared" si="3"/>
         <v>3.6999999999999997</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="20">
         <f t="shared" si="4"/>
         <v>1.0999999999999996</v>
       </c>
-      <c r="H23" s="26" t="str">
+      <c r="H23" s="21" t="str">
         <f t="shared" si="5"/>
         <v>Major Impairment</v>
       </c>
@@ -1335,27 +1330,27 @@
       <c r="B24" s="9">
         <v>9</v>
       </c>
-      <c r="C24" s="25">
+      <c r="C24" s="20">
         <f t="shared" si="0"/>
         <v>7.6</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="20">
         <f t="shared" si="1"/>
         <v>2.9</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="20">
         <f t="shared" si="2"/>
         <v>5.8</v>
       </c>
-      <c r="F24" s="25">
+      <c r="F24" s="20">
         <f t="shared" si="3"/>
         <v>4.6999999999999993</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="20">
         <f t="shared" si="4"/>
         <v>1.7999999999999998</v>
       </c>
-      <c r="H24" s="26" t="str">
+      <c r="H24" s="21" t="str">
         <f t="shared" si="5"/>
         <v>No Impairments</v>
       </c>
@@ -1367,27 +1362,27 @@
       <c r="B25" s="9">
         <v>11</v>
       </c>
-      <c r="C25" s="25">
+      <c r="C25" s="20">
         <f t="shared" si="0"/>
         <v>14.3</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="20">
         <f t="shared" si="1"/>
         <v>1.8</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="20">
         <f t="shared" si="2"/>
         <v>3.6</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F25" s="20">
         <f t="shared" si="3"/>
         <v>12.5</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="20">
         <f t="shared" si="4"/>
         <v>10.700000000000001</v>
       </c>
-      <c r="H25" s="26" t="str">
+      <c r="H25" s="21" t="str">
         <f t="shared" si="5"/>
         <v>Minor Impairment</v>
       </c>
@@ -1399,27 +1394,27 @@
       <c r="B26" s="9">
         <v>1</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="20">
         <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="20">
         <f t="shared" si="1"/>
         <v>1.3</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="20">
         <f t="shared" si="2"/>
         <v>2.6</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="20">
         <f t="shared" si="3"/>
         <v>9.9999999999999867E-2</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="20">
         <f t="shared" si="4"/>
         <v>-1.2000000000000002</v>
       </c>
-      <c r="H26" s="26" t="str">
+      <c r="H26" s="21" t="str">
         <f t="shared" si="5"/>
         <v>No Impairments</v>
       </c>
@@ -1428,74 +1423,83 @@
       <c r="A27" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="22">
         <f>SUM(B18:B26)</f>
         <v>47</v>
       </c>
-      <c r="C27" s="28">
-        <f>SUM(C18:C26)</f>
-        <v>61.6</v>
-      </c>
-      <c r="D27" s="28">
-        <f t="shared" ref="D27:G27" si="6">SUM(D18:D26)</f>
-        <v>18.899999999999999</v>
-      </c>
-      <c r="E27" s="28">
-        <f t="shared" si="6"/>
-        <v>37.799999999999997</v>
-      </c>
-      <c r="F27" s="28">
-        <f t="shared" si="6"/>
-        <v>42.699999999999996</v>
-      </c>
-      <c r="G27" s="28">
-        <f t="shared" si="6"/>
-        <v>23.8</v>
+      <c r="C27" s="20">
+        <f t="shared" si="0"/>
+        <v>62.6</v>
+      </c>
+      <c r="D27" s="20">
+        <f t="shared" si="1"/>
+        <v>11.4</v>
+      </c>
+      <c r="E27" s="20">
+        <f t="shared" si="2"/>
+        <v>22.8</v>
+      </c>
+      <c r="F27" s="20">
+        <f t="shared" si="3"/>
+        <v>51.2</v>
+      </c>
+      <c r="G27" s="20">
+        <f t="shared" si="4"/>
+        <v>39.799999999999997</v>
+      </c>
+      <c r="H27" s="21" t="str">
+        <f t="shared" si="5"/>
+        <v>Minor Impairment</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
+      <c r="A30" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="17" t="s">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="A33" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="23" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <conditionalFormatting sqref="B18:B26">
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <conditionalFormatting sqref="B18:B27">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$H18="Minor Impairment"</formula>
     </cfRule>
@@ -1514,6 +1518,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B27" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>